<commit_message>
Added the Disappeared Numbers in Go language
</commit_message>
<xml_diff>
--- a/170Problems.xlsx
+++ b/170Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\⠀\D&amp;A\The_170_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4AB3AE4-B080-4502-B2F0-3BB6CF1FE08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DB7A88-CF2E-45DB-AC68-B5A3D966D512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D66B45AE-877D-4D76-9BC7-59AA8D8FA9FB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D66B45AE-877D-4D76-9BC7-59AA8D8FA9FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,15 +34,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>1.. Arrays</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Contains Duplicate</t>
   </si>
   <si>
     <t>sort the array and check if the current item and the next are the same</t>
+  </si>
+  <si>
+    <t>1. Arrays</t>
+  </si>
+  <si>
+    <t>2. Arrays</t>
+  </si>
+  <si>
+    <t>3. Arrays</t>
+  </si>
+  <si>
+    <t>4. Arrays</t>
+  </si>
+  <si>
+    <t>Missing Number</t>
+  </si>
+  <si>
+    <t>Desappeared numbers</t>
+  </si>
+  <si>
+    <t>single Number</t>
+  </si>
+  <si>
+    <t>using xor with the given array and numbers from 1 .. N in result the missing number will get. Because 1^1 = 0.
+Another way is to calculate the sum of the array and the sum of the range and subtract.</t>
+  </si>
+  <si>
+    <t>using xor with the given array  1 .. N in result the missing number will get. Because 1^1 = 0.
+Another way is to calculate the sum of the array and the 2* sum of the range and subtract.</t>
   </si>
 </sst>
 </file>
@@ -84,9 +110,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38232C6-60ED-4B38-9E05-0273DBCA126F}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,13 +451,44 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
+    </row>
+    <row r="2" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish easy Dynamic Programming problems
</commit_message>
<xml_diff>
--- a/170Problems.xlsx
+++ b/170Problems.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\⠀\D&amp;A\170LeetcodeProblems\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\⠀\ComputerS\D&amp;A\170LeetcodeProblems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0092F4C-340D-4EB5-8B95-DC7770C909D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A73EAFB-437A-4D3E-8798-C63279EA7AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D66B45AE-877D-4D76-9BC7-59AA8D8FA9FB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Contains Duplicate</t>
   </si>
@@ -103,6 +103,25 @@
   <si>
     <t xml:space="preserve">Use current sum and max sum. Update max sum If current sum is the bigger then him. For the current sum if its negetive update to the current number.
 If not continue adding the current number to the sum. </t>
+  </si>
+  <si>
+    <t>8. Dynamic Programming</t>
+  </si>
+  <si>
+    <t>range sum</t>
+  </si>
+  <si>
+    <t>create a array to store the sums  of neghibors in the array and to find the range simply subtract the right index + 1 by the left index for the sum array</t>
+  </si>
+  <si>
+    <t>9. Dynamic Programming</t>
+  </si>
+  <si>
+    <t>Counting bits</t>
+  </si>
+  <si>
+    <t>The pattren of the 4 binary numbers is reapting in every Series. Every new "series" of number with this pattern have the same number of ones plus 1.
+The pattren always grows as the new series grows by *2.</t>
   </si>
 </sst>
 </file>
@@ -118,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,6 +147,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -144,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -156,9 +211,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38232C6-60ED-4B38-9E05-0273DBCA126F}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +546,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -498,7 +557,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -509,7 +568,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -520,7 +579,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -531,7 +590,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -542,7 +601,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -553,7 +612,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -561,6 +620,28 @@
       </c>
       <c r="C7" s="3" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resolved the hard question
</commit_message>
<xml_diff>
--- a/170Problems.xlsx
+++ b/170Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\⠀\ComputerS\D&amp;A\170LeetcodeProblems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A73EAFB-437A-4D3E-8798-C63279EA7AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304D2F5B-034D-420E-85F5-AB2080F2AC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D66B45AE-877D-4D76-9BC7-59AA8D8FA9FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D66B45AE-877D-4D76-9BC7-59AA8D8FA9FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -137,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,6 +183,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -199,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -218,6 +224,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,7 +544,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +605,7 @@
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -607,7 +616,7 @@
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -618,7 +627,7 @@
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -640,7 +649,7 @@
       <c r="B9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="12" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
First Fast & Slow problem
</commit_message>
<xml_diff>
--- a/170Problems.xlsx
+++ b/170Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\⠀\ComputerS\D&amp;A\170LeetcodeProblems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304D2F5B-034D-420E-85F5-AB2080F2AC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549A515E-B4A8-4BA4-8E41-4BC3E6EAAA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D66B45AE-877D-4D76-9BC7-59AA8D8FA9FB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D66B45AE-877D-4D76-9BC7-59AA8D8FA9FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Contains Duplicate</t>
   </si>
@@ -122,6 +122,15 @@
   <si>
     <t>The pattren of the 4 binary numbers is reapting in every Series. Every new "series" of number with this pattern have the same number of ones plus 1.
 The pattren always grows as the new series grows by *2.</t>
+  </si>
+  <si>
+    <t>10. Fast &amp; Slow Pointers</t>
+  </si>
+  <si>
+    <t>Has Cycle</t>
+  </si>
+  <si>
+    <t>Go throw the linked list with fast &amp; slow pointer. If they both point to the same node then there is a cycle</t>
   </si>
 </sst>
 </file>
@@ -188,7 +197,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38232C6-60ED-4B38-9E05-0273DBCA126F}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,6 +662,17 @@
         <v>26</v>
       </c>
     </row>
+    <row r="10" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
almost finish all fast & slow pointers
</commit_message>
<xml_diff>
--- a/170Problems.xlsx
+++ b/170Problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\⠀\ComputerS\D&amp;A\170LeetcodeProblems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549A515E-B4A8-4BA4-8E41-4BC3E6EAAA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442AF700-54CF-4386-A1EA-3C8DDF0C1DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D66B45AE-877D-4D76-9BC7-59AA8D8FA9FB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Contains Duplicate</t>
   </si>
@@ -131,6 +131,35 @@
   </si>
   <si>
     <t>Go throw the linked list with fast &amp; slow pointer. If they both point to the same node then there is a cycle</t>
+  </si>
+  <si>
+    <t>11. Fast &amp; Slow Pointers</t>
+  </si>
+  <si>
+    <t>middleNode</t>
+  </si>
+  <si>
+    <t>Go throw the linked list with fast &amp; slow pointer. The fast pointer is going two nodes at one jump and the slow one node at the time.
+Meaning when the fast pointer gets to the end the slow pointer will be doing half of the way hence middle.</t>
+  </si>
+  <si>
+    <t>12. Fast &amp;Slow Pointers</t>
+  </si>
+  <si>
+    <t>Palindrome Linked list</t>
+  </si>
+  <si>
+    <t>find the middle point by question (11) and save the values in array. Compare the rest of the linked list to the array's values in reverse</t>
+  </si>
+  <si>
+    <t>13. Fast &amp; Slow Pointers</t>
+  </si>
+  <si>
+    <t>remove elements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If we have a head then call stack to the recursive function. After getting to the end check in reverse if the current value need to be removed if it is remove it.
+Return the head and close this function call. </t>
   </si>
 </sst>
 </file>
@@ -146,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,6 +227,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -214,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -234,6 +269,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -550,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38232C6-60ED-4B38-9E05-0273DBCA126F}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,6 +711,39 @@
         <v>29</v>
       </c>
     </row>
+    <row r="11" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added two more problems
</commit_message>
<xml_diff>
--- a/170Problems.xlsx
+++ b/170Problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\⠀\ComputerS\D&amp;A\170LeetcodeProblems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442AF700-54CF-4386-A1EA-3C8DDF0C1DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8FD5F7-0739-48F9-99F8-D7055506D2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D66B45AE-877D-4D76-9BC7-59AA8D8FA9FB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Contains Duplicate</t>
   </si>
@@ -160,6 +160,15 @@
   <si>
     <t xml:space="preserve">If we have a head then call stack to the recursive function. After getting to the end check in reverse if the current value need to be removed if it is remove it.
 Return the head and close this function call. </t>
+  </si>
+  <si>
+    <t>14. Fast &amp; Slow Pointers</t>
+  </si>
+  <si>
+    <t>Remove duplicates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travers through the linked list. If curr.next </t>
   </si>
 </sst>
 </file>
@@ -588,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38232C6-60ED-4B38-9E05-0273DBCA126F}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,6 +753,17 @@
         <v>38</v>
       </c>
     </row>
+    <row r="14" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added 4 more solutions
</commit_message>
<xml_diff>
--- a/170Problems.xlsx
+++ b/170Problems.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\⠀\ComputerS\D&amp;A\170LeetcodeProblems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8FD5F7-0739-48F9-99F8-D7055506D2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2115048E-EECB-47D5-B564-F63BFFD28858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D66B45AE-877D-4D76-9BC7-59AA8D8FA9FB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Contains Duplicate</t>
   </si>
@@ -152,9 +152,6 @@
     <t>find the middle point by question (11) and save the values in array. Compare the rest of the linked list to the array's values in reverse</t>
   </si>
   <si>
-    <t>13. Fast &amp; Slow Pointers</t>
-  </si>
-  <si>
     <t>remove elements</t>
   </si>
   <si>
@@ -162,13 +159,61 @@
 Return the head and close this function call. </t>
   </si>
   <si>
-    <t>14. Fast &amp; Slow Pointers</t>
-  </si>
-  <si>
     <t>Remove duplicates</t>
   </si>
   <si>
-    <t xml:space="preserve">Travers through the linked list. If curr.next </t>
+    <t>Travers through the linked list. If curr.next == curr then skip over curr.next.</t>
+  </si>
+  <si>
+    <t>15. Linked list</t>
+  </si>
+  <si>
+    <t>14. Linked List</t>
+  </si>
+  <si>
+    <t>13. Linked List</t>
+  </si>
+  <si>
+    <t>reverse a linked list</t>
+  </si>
+  <si>
+    <t>Travers through the linked list. Save temp var for curr.next and update the curr.Next to the prev node and update curr and prev. At last return the prev</t>
+  </si>
+  <si>
+    <t>16. Linked list &amp; two Ptrs</t>
+  </si>
+  <si>
+    <t>merge two sorted lists</t>
+  </si>
+  <si>
+    <t>go throw both lists and have one pointer for each list then check which node have the smallest value and add it to the new list, (increment the list pointer)</t>
+  </si>
+  <si>
+    <t>17. two pointers</t>
+  </si>
+  <si>
+    <t>binary search</t>
+  </si>
+  <si>
+    <t>use high low middle pointers if the middle is the target index then return it and if we don't find return -1 (low &lt;= high while loop)</t>
+  </si>
+  <si>
+    <t>18. array</t>
+  </si>
+  <si>
+    <t>smallest letter bigger then target</t>
+  </si>
+  <si>
+    <t>return the first letter that bigger then the target if not found then return the first letter</t>
+  </si>
+  <si>
+    <t>find the peak of a mountain</t>
+  </si>
+  <si>
+    <t>find the max of the array. Do the follow up.</t>
+  </si>
+  <si>
+    <t>19. Array &amp; binary search</t>
   </si>
 </sst>
 </file>
@@ -258,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -283,6 +328,10 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38232C6-60ED-4B38-9E05-0273DBCA126F}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,24 +793,79 @@
     </row>
     <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="13" t="s">
+    </row>
+    <row r="14" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C14" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="5" t="s">
+    </row>
+    <row r="15" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>41</v>
+      <c r="B15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
did 2 new problems in trees and redo the mountain with log n complexity and understand way better binary search
</commit_message>
<xml_diff>
--- a/170Problems.xlsx
+++ b/170Problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\⠀\ComputerS\D&amp;A\170LeetcodeProblems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2115048E-EECB-47D5-B564-F63BFFD28858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2A9E41-95A3-489C-8B22-EED67F2EB733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D66B45AE-877D-4D76-9BC7-59AA8D8FA9FB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Contains Duplicate</t>
   </si>
@@ -210,10 +210,28 @@
     <t>find the peak of a mountain</t>
   </si>
   <si>
-    <t>find the max of the array. Do the follow up.</t>
-  </si>
-  <si>
     <t>19. Array &amp; binary search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">find the max of the array. Binary search with a little change for the spacific problem differente condition </t>
+  </si>
+  <si>
+    <t>20. BFS</t>
+  </si>
+  <si>
+    <t>Average of levels in binary tree</t>
+  </si>
+  <si>
+    <t>use a queue to store the current level of the tree. Every time that we dequeue the current nodes add their left and right. If they are not null</t>
+  </si>
+  <si>
+    <t>21. BFS</t>
+  </si>
+  <si>
+    <t>Minimum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>travers through the tree in BFS using queue and two loops. And return the first leaf's depth. (level + 1)</t>
   </si>
 </sst>
 </file>
@@ -646,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38232C6-60ED-4B38-9E05-0273DBCA126F}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,13 +877,35 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>